<commit_message>
Making changes in the graph and Adding final excel sheet
</commit_message>
<xml_diff>
--- a/MBIST input test run output/Changes In HTM Parameters.xlsx
+++ b/MBIST input test run output/Changes In HTM Parameters.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\source\repos\neocortexapi-classification\MBIST input test run output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB150F95-6364-40F7-BD41-1CA95E79427E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3B6D607D-F578-41B6-BEE1-C14BD1182640}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="67">
   <si>
     <t>Local Area Density</t>
   </si>
@@ -105,26 +105,151 @@
     <t>Exp 5</t>
   </si>
   <si>
-    <t>Exp</t>
-  </si>
-  <si>
     <t>Exp 1.</t>
   </si>
   <si>
     <t>Exp 2.</t>
   </si>
   <si>
-    <t>Exp 201</t>
+    <t xml:space="preserve">Exp 20 </t>
+  </si>
+  <si>
+    <t>Exp 21</t>
+  </si>
+  <si>
+    <t>exp 22</t>
+  </si>
+  <si>
+    <t>Exp 22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exp 23 </t>
+  </si>
+  <si>
+    <t>Exp 23</t>
+  </si>
+  <si>
+    <t>Exp 25</t>
+  </si>
+  <si>
+    <t>Exp 27</t>
+  </si>
+  <si>
+    <t>Exp 28</t>
+  </si>
+  <si>
+    <t>Exp 30</t>
+  </si>
+  <si>
+    <t>Exp 31</t>
+  </si>
+  <si>
+    <t>Exp 32</t>
+  </si>
+  <si>
+    <t>Exp 33</t>
+  </si>
+  <si>
+    <t>Exp 34</t>
+  </si>
+  <si>
+    <t>Exp 35</t>
+  </si>
+  <si>
+    <t>Exp 36</t>
+  </si>
+  <si>
+    <t>Exp 37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exp 38 </t>
+  </si>
+  <si>
+    <t>Exp 39</t>
+  </si>
+  <si>
+    <t>Exp 40</t>
+  </si>
+  <si>
+    <t>Exp 41</t>
+  </si>
+  <si>
+    <t>Exp 42</t>
+  </si>
+  <si>
+    <t>Exp 43</t>
+  </si>
+  <si>
+    <t>Exp 44</t>
+  </si>
+  <si>
+    <t>Exp 45</t>
+  </si>
+  <si>
+    <t>Exp 46</t>
+  </si>
+  <si>
+    <t>Exp 47</t>
+  </si>
+  <si>
+    <t>Exp 48</t>
+  </si>
+  <si>
+    <t>Exp 49</t>
+  </si>
+  <si>
+    <t>Exp 50</t>
+  </si>
+  <si>
+    <t>Image Dimension</t>
+  </si>
+  <si>
+    <t>Column Dimension</t>
+  </si>
+  <si>
+    <t>Micro</t>
+  </si>
+  <si>
+    <t>Micro wrt other image</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data Set </t>
+  </si>
+  <si>
+    <t>8,5,6</t>
+  </si>
+  <si>
+    <t>5,4,3</t>
+  </si>
+  <si>
+    <t>9,1,0</t>
+  </si>
+  <si>
+    <t>Exp 38</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -171,13 +296,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -460,10 +592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:N50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -473,10 +605,15 @@
     <col min="3" max="3" width="16.88671875" customWidth="1"/>
     <col min="4" max="4" width="21.44140625" customWidth="1"/>
     <col min="5" max="5" width="28.33203125" customWidth="1"/>
-    <col min="6" max="6" width="21.33203125" customWidth="1"/>
+    <col min="6" max="6" width="28.33203125" style="5" customWidth="1"/>
+    <col min="7" max="7" width="21.33203125" customWidth="1"/>
+    <col min="8" max="8" width="15.5546875" customWidth="1"/>
+    <col min="9" max="9" width="18" customWidth="1"/>
+    <col min="13" max="13" width="20.88671875" customWidth="1"/>
+    <col min="14" max="14" width="28.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -492,11 +629,31 @@
       <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H1" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>21</v>
       </c>
@@ -512,13 +669,37 @@
       <c r="E2" s="3">
         <v>-1</v>
       </c>
-      <c r="F2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F2" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2">
+        <v>28</v>
+      </c>
+      <c r="I2">
+        <v>32</v>
+      </c>
+      <c r="J2">
+        <v>100</v>
+      </c>
+      <c r="K2">
+        <v>99.68</v>
+      </c>
+      <c r="L2">
+        <v>100</v>
+      </c>
+      <c r="M2">
+        <v>97.81</v>
+      </c>
+      <c r="N2">
+        <v>98.24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B3" s="3">
         <v>0.1</v>
@@ -532,11 +713,35 @@
       <c r="E3" s="3">
         <v>-1</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H3">
+        <v>28</v>
+      </c>
+      <c r="I3">
+        <v>32</v>
+      </c>
+      <c r="J3">
+        <v>99.21</v>
+      </c>
+      <c r="K3">
+        <v>99.6</v>
+      </c>
+      <c r="L3">
+        <v>98.43</v>
+      </c>
+      <c r="M3">
+        <v>97.85</v>
+      </c>
+      <c r="N3">
+        <v>98.24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>22</v>
       </c>
@@ -552,11 +757,35 @@
       <c r="E4" s="3">
         <v>-1</v>
       </c>
-      <c r="F4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F4" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="5">
+        <v>28</v>
+      </c>
+      <c r="I4" s="5">
+        <v>32</v>
+      </c>
+      <c r="J4">
+        <v>98.82</v>
+      </c>
+      <c r="K4">
+        <v>99.41</v>
+      </c>
+      <c r="L4">
+        <v>98.62</v>
+      </c>
+      <c r="M4">
+        <v>97.65</v>
+      </c>
+      <c r="N4">
+        <v>98.43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>23</v>
       </c>
@@ -572,11 +801,35 @@
       <c r="E5" s="3">
         <v>-1</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H5" s="5">
+        <v>28</v>
+      </c>
+      <c r="I5" s="5">
+        <v>32</v>
+      </c>
+      <c r="J5">
+        <v>99.41</v>
+      </c>
+      <c r="K5">
+        <v>100</v>
+      </c>
+      <c r="L5">
+        <v>99.41</v>
+      </c>
+      <c r="M5">
+        <v>99.022999999999996</v>
+      </c>
+      <c r="N5">
+        <v>99.02</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>24</v>
       </c>
@@ -592,11 +845,35 @@
       <c r="E6" s="3">
         <v>-1</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G6" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H6" s="5">
+        <v>28</v>
+      </c>
+      <c r="I6" s="5">
+        <v>32</v>
+      </c>
+      <c r="J6">
+        <v>99.51</v>
+      </c>
+      <c r="K6">
+        <v>100</v>
+      </c>
+      <c r="L6">
+        <v>99.608999999999995</v>
+      </c>
+      <c r="M6">
+        <v>99.9</v>
+      </c>
+      <c r="N6">
+        <v>99.41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>25</v>
       </c>
@@ -612,11 +889,35 @@
       <c r="E7" s="3">
         <v>-1</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G7" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H7" s="5">
+        <v>28</v>
+      </c>
+      <c r="I7" s="5">
+        <v>32</v>
+      </c>
+      <c r="J7">
+        <v>99.8</v>
+      </c>
+      <c r="K7">
+        <v>100</v>
+      </c>
+      <c r="L7">
+        <v>99.8</v>
+      </c>
+      <c r="M7">
+        <v>99.8</v>
+      </c>
+      <c r="N7">
+        <v>98.8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>5</v>
       </c>
@@ -632,11 +933,35 @@
       <c r="E8" s="3">
         <v>-1</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G8" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H8" s="5">
+        <v>28</v>
+      </c>
+      <c r="I8" s="5">
+        <v>32</v>
+      </c>
+      <c r="J8">
+        <v>99.47</v>
+      </c>
+      <c r="K8">
+        <v>99.47</v>
+      </c>
+      <c r="L8">
+        <v>98.56</v>
+      </c>
+      <c r="M8">
+        <v>98.43</v>
+      </c>
+      <c r="N8">
+        <v>98.69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>6</v>
       </c>
@@ -652,11 +977,35 @@
       <c r="E9" s="3">
         <v>-1</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G9" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H9" s="5">
+        <v>28</v>
+      </c>
+      <c r="I9" s="5">
+        <v>32</v>
+      </c>
+      <c r="J9">
+        <v>99.75</v>
+      </c>
+      <c r="K9">
+        <v>99.63</v>
+      </c>
+      <c r="L9">
+        <v>98.9</v>
+      </c>
+      <c r="M9">
+        <v>98.74</v>
+      </c>
+      <c r="N9">
+        <v>98.95</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
@@ -672,11 +1021,35 @@
       <c r="E10" s="3">
         <v>-1</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H10" s="5">
+        <v>28</v>
+      </c>
+      <c r="I10" s="5">
+        <v>32</v>
+      </c>
+      <c r="J10">
+        <v>99.54</v>
+      </c>
+      <c r="K10">
+        <v>99.77</v>
+      </c>
+      <c r="L10">
+        <v>99.31</v>
+      </c>
+      <c r="M10">
+        <v>99.42</v>
+      </c>
+      <c r="N10">
+        <v>99.08</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
@@ -692,11 +1065,35 @@
       <c r="E11" s="3">
         <v>-1</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G11" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H11" s="5">
+        <v>28</v>
+      </c>
+      <c r="I11" s="5">
+        <v>32</v>
+      </c>
+      <c r="J11">
+        <v>99.566000000000003</v>
+      </c>
+      <c r="K11">
+        <v>99.89</v>
+      </c>
+      <c r="L11">
+        <v>99.67</v>
+      </c>
+      <c r="M11">
+        <v>99.45</v>
+      </c>
+      <c r="N11">
+        <v>99.56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
@@ -712,11 +1109,35 @@
       <c r="E12" s="3">
         <v>-1</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G12" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H12" s="5">
+        <v>28</v>
+      </c>
+      <c r="I12" s="5">
+        <v>32</v>
+      </c>
+      <c r="J12">
+        <v>99.79</v>
+      </c>
+      <c r="K12">
+        <v>99.79</v>
+      </c>
+      <c r="L12">
+        <v>99.48</v>
+      </c>
+      <c r="M12">
+        <v>99.69</v>
+      </c>
+      <c r="N12">
+        <v>99.587999999999994</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>12</v>
       </c>
@@ -732,11 +1153,35 @@
       <c r="E13" s="3">
         <v>-1</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G13" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H13" s="5">
+        <v>28</v>
+      </c>
+      <c r="I13" s="5">
+        <v>32</v>
+      </c>
+      <c r="J13">
+        <v>99.21</v>
+      </c>
+      <c r="K13">
+        <v>98.43</v>
+      </c>
+      <c r="L13">
+        <v>98.43</v>
+      </c>
+      <c r="M13">
+        <v>97.65</v>
+      </c>
+      <c r="N13">
+        <v>98.04</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
@@ -752,11 +1197,35 @@
       <c r="E14" s="3">
         <v>-1</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G14" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H14" s="5">
+        <v>28</v>
+      </c>
+      <c r="I14" s="5">
+        <v>32</v>
+      </c>
+      <c r="J14">
+        <v>98.75</v>
+      </c>
+      <c r="K14">
+        <v>98.57</v>
+      </c>
+      <c r="L14">
+        <v>98.22</v>
+      </c>
+      <c r="M14">
+        <v>98.04</v>
+      </c>
+      <c r="N14">
+        <v>98.57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>14</v>
       </c>
@@ -772,11 +1241,35 @@
       <c r="E15" s="3">
         <v>-1</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H15" s="5">
+        <v>28</v>
+      </c>
+      <c r="I15" s="5">
+        <v>32</v>
+      </c>
+      <c r="J15">
+        <v>99.34</v>
+      </c>
+      <c r="K15">
+        <v>99.67</v>
+      </c>
+      <c r="L15">
+        <v>98.37</v>
+      </c>
+      <c r="M15">
+        <v>98.2</v>
+      </c>
+      <c r="N15">
+        <v>98.37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>15</v>
       </c>
@@ -792,11 +1285,35 @@
       <c r="E16" s="3">
         <v>-1</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G16" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H16" s="5">
+        <v>28</v>
+      </c>
+      <c r="I16" s="5">
+        <v>32</v>
+      </c>
+      <c r="J16">
+        <v>98.49</v>
+      </c>
+      <c r="K16">
+        <v>99.69</v>
+      </c>
+      <c r="L16">
+        <v>98.94</v>
+      </c>
+      <c r="M16">
+        <v>98.04</v>
+      </c>
+      <c r="N16">
+        <v>98.04</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>16</v>
       </c>
@@ -812,11 +1329,35 @@
       <c r="E17" s="3">
         <v>-1</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G17" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H17" s="5">
+        <v>28</v>
+      </c>
+      <c r="I17" s="5">
+        <v>32</v>
+      </c>
+      <c r="J17">
+        <v>99.16</v>
+      </c>
+      <c r="K17">
+        <v>99.44</v>
+      </c>
+      <c r="L17">
+        <v>98.74</v>
+      </c>
+      <c r="M17">
+        <v>98.6</v>
+      </c>
+      <c r="N17">
+        <v>98.88</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>17</v>
       </c>
@@ -832,11 +1373,35 @@
       <c r="E18" s="3">
         <v>-1</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F18" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G18" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H18" s="5">
+        <v>28</v>
+      </c>
+      <c r="I18" s="5">
+        <v>32</v>
+      </c>
+      <c r="J18">
+        <v>99.21</v>
+      </c>
+      <c r="K18">
+        <v>99.73</v>
+      </c>
+      <c r="L18">
+        <v>98.82</v>
+      </c>
+      <c r="M18">
+        <v>98.56</v>
+      </c>
+      <c r="N18">
+        <v>99.08</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>18</v>
       </c>
@@ -852,51 +1417,1370 @@
       <c r="E19" s="3">
         <v>-1</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G19" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H19" s="5">
+        <v>28</v>
+      </c>
+      <c r="I19" s="5">
+        <v>32</v>
+      </c>
+      <c r="J19">
+        <v>98.77</v>
+      </c>
+      <c r="K19">
+        <v>99.75</v>
+      </c>
+      <c r="L19">
+        <v>99.02</v>
+      </c>
+      <c r="M19">
+        <v>98.77</v>
+      </c>
+      <c r="N19">
+        <v>99.02</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="3">
+        <v>1</v>
+      </c>
+      <c r="C20" s="3">
+        <v>20</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G20" t="s">
+        <v>19</v>
+      </c>
+      <c r="H20" s="5">
+        <v>28</v>
+      </c>
+      <c r="I20" s="5">
+        <v>32</v>
+      </c>
+      <c r="J20">
+        <v>100</v>
+      </c>
+      <c r="K20">
+        <v>100</v>
+      </c>
+      <c r="L20">
+        <v>100</v>
+      </c>
+      <c r="M20">
+        <v>100</v>
+      </c>
+      <c r="N20">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="C21" s="3">
+        <v>20</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E21" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G21" t="s">
+        <v>20</v>
+      </c>
+      <c r="H21" s="5">
+        <v>28</v>
+      </c>
+      <c r="I21" s="5">
+        <v>32</v>
+      </c>
+      <c r="J21">
+        <v>100</v>
+      </c>
+      <c r="K21">
+        <v>100</v>
+      </c>
+      <c r="L21">
+        <v>100</v>
+      </c>
+      <c r="M21">
+        <v>99.01</v>
+      </c>
+      <c r="N21">
+        <v>96.07</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" s="3">
+        <v>0.15</v>
+      </c>
+      <c r="C22" s="3">
+        <v>20</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E22" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G22" t="s">
+        <v>28</v>
+      </c>
+      <c r="H22" s="5">
+        <v>28</v>
+      </c>
+      <c r="I22" s="5">
+        <v>32</v>
+      </c>
+      <c r="J22">
+        <v>100</v>
+      </c>
+      <c r="K22">
+        <v>99.35</v>
+      </c>
+      <c r="L22">
+        <v>100</v>
+      </c>
+      <c r="M22">
+        <v>95.453999999999994</v>
+      </c>
+      <c r="N22">
+        <v>92.85</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B23" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="C23" s="3">
+        <v>20</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E23" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G23" t="s">
+        <v>29</v>
+      </c>
+      <c r="H23" s="5">
+        <v>28</v>
+      </c>
+      <c r="I23" s="5">
+        <v>32</v>
+      </c>
+      <c r="J23">
+        <v>100</v>
+      </c>
+      <c r="K23">
+        <v>99.02</v>
+      </c>
+      <c r="L23">
+        <v>100</v>
+      </c>
+      <c r="M23">
+        <v>99.02</v>
+      </c>
+      <c r="N23">
+        <v>94.63</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="C24" s="3">
+        <v>20</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E24" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G24" t="s">
+        <v>31</v>
+      </c>
+      <c r="H24" s="5">
+        <v>28</v>
+      </c>
+      <c r="I24" s="5">
+        <v>32</v>
+      </c>
+      <c r="J24">
+        <v>100</v>
+      </c>
+      <c r="K24">
+        <v>98.04</v>
+      </c>
+      <c r="L24">
+        <v>100</v>
+      </c>
+      <c r="M24">
+        <v>98.43</v>
+      </c>
+      <c r="N24">
+        <v>96.87</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="C25" s="3">
+        <v>20</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E25" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G25" t="s">
+        <v>33</v>
+      </c>
+      <c r="H25" s="5">
+        <v>28</v>
+      </c>
+      <c r="I25" s="5">
+        <v>32</v>
+      </c>
+      <c r="J25">
+        <v>100</v>
+      </c>
+      <c r="K25">
+        <v>99.69</v>
+      </c>
+      <c r="L25">
+        <v>100</v>
+      </c>
+      <c r="M25">
+        <v>98.69</v>
+      </c>
+      <c r="N25">
+        <v>96.74</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="C26" s="3">
+        <v>20</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E26" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H26" s="5">
+        <v>28</v>
+      </c>
+      <c r="I26" s="5">
+        <v>32</v>
+      </c>
+      <c r="J26">
+        <v>100</v>
+      </c>
+      <c r="K26">
+        <v>99.02</v>
+      </c>
+      <c r="L26">
+        <v>100</v>
+      </c>
+      <c r="M26">
+        <v>98.04</v>
+      </c>
+      <c r="N26">
+        <v>96.82</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C27" s="3">
+        <v>20</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E27" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H27" s="5">
+        <v>28</v>
+      </c>
+      <c r="I27" s="5">
+        <v>32</v>
+      </c>
+      <c r="J27">
+        <v>100</v>
+      </c>
+      <c r="K27">
+        <v>99.41</v>
+      </c>
+      <c r="L27">
+        <v>100</v>
+      </c>
+      <c r="M27">
+        <v>99.41</v>
+      </c>
+      <c r="N27">
+        <v>98.24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" s="3">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="C28" s="3">
+        <v>20</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E28" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="H28" s="5">
+        <v>28</v>
+      </c>
+      <c r="I28" s="5">
+        <v>32</v>
+      </c>
+      <c r="J28">
+        <v>100</v>
+      </c>
+      <c r="K28">
+        <v>99.46</v>
+      </c>
+      <c r="L28">
+        <v>100</v>
+      </c>
+      <c r="M28">
+        <v>99.46</v>
+      </c>
+      <c r="N28">
+        <v>98.57</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B29" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="C29" s="3">
+        <v>20</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E29" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H29" s="5">
+        <v>28</v>
+      </c>
+      <c r="I29" s="5">
+        <v>32</v>
+      </c>
+      <c r="J29">
+        <v>100</v>
+      </c>
+      <c r="K29">
+        <v>99.51</v>
+      </c>
+      <c r="L29">
+        <v>100</v>
+      </c>
+      <c r="M29">
+        <v>99.34</v>
+      </c>
+      <c r="N29">
+        <v>98.37</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B30" s="3">
+        <v>0.65</v>
+      </c>
+      <c r="C30" s="3">
+        <v>20</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E30" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G30" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H30" s="5">
+        <v>28</v>
+      </c>
+      <c r="I30" s="5">
+        <v>32</v>
+      </c>
+      <c r="J30">
+        <v>100</v>
+      </c>
+      <c r="K30">
+        <v>99.69</v>
+      </c>
+      <c r="L30">
+        <v>100</v>
+      </c>
+      <c r="M30">
+        <v>99.58</v>
+      </c>
+      <c r="N30">
+        <v>98.64</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A31" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="C31" s="3">
+        <v>20</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E31" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="H31" s="5">
+        <v>28</v>
+      </c>
+      <c r="I31" s="5">
+        <v>32</v>
+      </c>
+      <c r="J31">
+        <v>100</v>
+      </c>
+      <c r="K31">
+        <v>99.44</v>
+      </c>
+      <c r="L31">
+        <v>100</v>
+      </c>
+      <c r="M31">
+        <v>99.58</v>
+      </c>
+      <c r="N31">
+        <v>98.88</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A32" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B32" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="C32" s="3">
+        <v>20</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E32" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="H32" s="5">
+        <v>28</v>
+      </c>
+      <c r="I32" s="5">
+        <v>32</v>
+      </c>
+      <c r="J32">
+        <v>100</v>
+      </c>
+      <c r="K32">
+        <v>99.73</v>
+      </c>
+      <c r="L32">
+        <v>100</v>
+      </c>
+      <c r="M32">
+        <v>99.38</v>
+      </c>
+      <c r="N32">
+        <v>98.82</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A33" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B33" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="C33" s="3">
+        <v>20</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E33" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H33" s="5">
+        <v>28</v>
+      </c>
+      <c r="I33" s="5">
+        <v>32</v>
+      </c>
+      <c r="J33">
+        <v>100</v>
+      </c>
+      <c r="K33">
+        <v>99.87</v>
+      </c>
+      <c r="L33">
+        <v>100</v>
+      </c>
+      <c r="M33">
+        <v>99.87</v>
+      </c>
+      <c r="N33">
+        <v>99.14</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A34" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B34" s="3">
         <v>0.85</v>
       </c>
-      <c r="C20" s="3">
-        <v>40</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E20" s="3">
-        <v>-1</v>
-      </c>
-      <c r="F20" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B21" s="3">
+      <c r="C34" s="3">
+        <v>20</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E34" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H34" s="5">
+        <v>28</v>
+      </c>
+      <c r="I34">
+        <v>32</v>
+      </c>
+      <c r="J34">
+        <v>100</v>
+      </c>
+      <c r="K34">
+        <v>100</v>
+      </c>
+      <c r="L34">
+        <v>100</v>
+      </c>
+      <c r="M34">
+        <v>99.89</v>
+      </c>
+      <c r="N34">
+        <v>99.78</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A35" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B35" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="C35" s="3">
+        <v>20</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E35" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="H35" s="5">
+        <v>28</v>
+      </c>
+      <c r="I35">
+        <v>64</v>
+      </c>
+      <c r="J35">
+        <v>100</v>
+      </c>
+      <c r="K35">
+        <v>100</v>
+      </c>
+      <c r="L35">
+        <v>100</v>
+      </c>
+      <c r="M35">
+        <v>99.89</v>
+      </c>
+      <c r="N35">
+        <v>99.78</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A36" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B36" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="C36" s="3">
+        <v>20</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E36" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="H36" s="5">
+        <v>28</v>
+      </c>
+      <c r="I36">
+        <v>64</v>
+      </c>
+      <c r="J36">
+        <v>100</v>
+      </c>
+      <c r="K36">
+        <v>100</v>
+      </c>
+      <c r="L36">
+        <v>100</v>
+      </c>
+      <c r="M36">
+        <v>99.89</v>
+      </c>
+      <c r="N36">
+        <v>99.79</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A37" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B37" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="C37" s="3">
+        <v>30</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E37" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="H37" s="5">
+        <v>28</v>
+      </c>
+      <c r="I37">
+        <v>64</v>
+      </c>
+      <c r="J37">
+        <v>100</v>
+      </c>
+      <c r="K37">
+        <v>96.07</v>
+      </c>
+      <c r="L37">
+        <v>100</v>
+      </c>
+      <c r="M37">
+        <v>98.03</v>
+      </c>
+      <c r="N37">
+        <v>92.156000000000006</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A38" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B38" s="3">
+        <v>0.15</v>
+      </c>
+      <c r="C38" s="3">
+        <v>30</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E38" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G38" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="H38" s="5">
+        <v>28</v>
+      </c>
+      <c r="I38">
+        <v>64</v>
+      </c>
+      <c r="J38">
+        <v>100</v>
+      </c>
+      <c r="K38">
+        <v>98.04</v>
+      </c>
+      <c r="L38">
+        <v>100</v>
+      </c>
+      <c r="M38">
+        <v>97.39</v>
+      </c>
+      <c r="N38">
+        <v>95.92</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A39" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B39" s="3">
         <v>0.2</v>
       </c>
-      <c r="C21" s="3">
-        <v>40</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E21" s="3">
-        <v>-1</v>
-      </c>
-      <c r="F21" t="s">
-        <v>20</v>
+      <c r="C39" s="3">
+        <v>30</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E39" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="H39" s="5">
+        <v>28</v>
+      </c>
+      <c r="I39">
+        <v>64</v>
+      </c>
+      <c r="J39">
+        <v>100</v>
+      </c>
+      <c r="K39">
+        <v>98.29</v>
+      </c>
+      <c r="L39">
+        <v>100</v>
+      </c>
+      <c r="M39">
+        <v>98.16</v>
+      </c>
+      <c r="N39">
+        <v>95.72</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A40" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B40" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="C40" s="3">
+        <v>30</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E40" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G40" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="H40" s="5">
+        <v>28</v>
+      </c>
+      <c r="I40">
+        <v>64</v>
+      </c>
+      <c r="J40">
+        <v>100</v>
+      </c>
+      <c r="K40">
+        <v>98.92</v>
+      </c>
+      <c r="L40">
+        <v>100</v>
+      </c>
+      <c r="M40">
+        <v>98.24</v>
+      </c>
+      <c r="N40">
+        <v>96.38</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A41" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B41" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="C41" s="3">
+        <v>30</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E41" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G41" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="H41" s="5">
+        <v>28</v>
+      </c>
+      <c r="I41">
+        <v>64</v>
+      </c>
+      <c r="J41">
+        <v>100</v>
+      </c>
+      <c r="K41">
+        <v>98.94</v>
+      </c>
+      <c r="L41">
+        <v>100</v>
+      </c>
+      <c r="M41">
+        <v>98.2</v>
+      </c>
+      <c r="N41">
+        <v>96.9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A42" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B42" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="C42" s="3">
+        <v>30</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E42" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G42" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="H42" s="5">
+        <v>28</v>
+      </c>
+      <c r="I42" s="5">
+        <v>64</v>
+      </c>
+      <c r="J42">
+        <v>100</v>
+      </c>
+      <c r="K42">
+        <v>99.09</v>
+      </c>
+      <c r="L42">
+        <v>100</v>
+      </c>
+      <c r="M42">
+        <v>98.53</v>
+      </c>
+      <c r="N42">
+        <v>97.35</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A43" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B43" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="C43" s="3">
+        <v>30</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E43" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G43" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="H43" s="5">
+        <v>28</v>
+      </c>
+      <c r="I43" s="5">
+        <v>64</v>
+      </c>
+      <c r="J43">
+        <v>100</v>
+      </c>
+      <c r="K43">
+        <v>99.08</v>
+      </c>
+      <c r="L43">
+        <v>100</v>
+      </c>
+      <c r="M43">
+        <v>98.71</v>
+      </c>
+      <c r="N43">
+        <v>97.49</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A44" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B44" s="3">
+        <v>0.45</v>
+      </c>
+      <c r="C44" s="3">
+        <v>30</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E44" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G44" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="H44" s="5">
+        <v>28</v>
+      </c>
+      <c r="I44" s="5">
+        <v>64</v>
+      </c>
+      <c r="J44">
+        <v>100</v>
+      </c>
+      <c r="K44">
+        <v>99.24</v>
+      </c>
+      <c r="L44">
+        <v>100</v>
+      </c>
+      <c r="M44">
+        <v>99.076999999999998</v>
+      </c>
+      <c r="N44">
+        <v>97.23</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A45" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B45" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C45" s="3">
+        <v>30</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E45" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G45" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H45" s="5">
+        <v>28</v>
+      </c>
+      <c r="I45" s="5">
+        <v>64</v>
+      </c>
+      <c r="J45">
+        <v>100</v>
+      </c>
+      <c r="K45">
+        <v>99.36</v>
+      </c>
+      <c r="L45">
+        <v>100</v>
+      </c>
+      <c r="M45">
+        <v>99.16</v>
+      </c>
+      <c r="N45">
+        <v>97.85</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A46" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B46" s="3">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="C46" s="3">
+        <v>30</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E46" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G46" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="H46" s="5">
+        <v>28</v>
+      </c>
+      <c r="I46" s="5">
+        <v>64</v>
+      </c>
+      <c r="J46">
+        <v>100</v>
+      </c>
+      <c r="K46">
+        <v>99.51</v>
+      </c>
+      <c r="L46">
+        <v>100</v>
+      </c>
+      <c r="M46">
+        <v>99.24</v>
+      </c>
+      <c r="N46">
+        <v>98.35</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A47" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B47" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="C47" s="3">
+        <v>30</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E47" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G47" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="H47" s="5">
+        <v>28</v>
+      </c>
+      <c r="I47" s="5">
+        <v>64</v>
+      </c>
+      <c r="J47">
+        <v>100</v>
+      </c>
+      <c r="K47">
+        <v>99.51</v>
+      </c>
+      <c r="L47">
+        <v>100</v>
+      </c>
+      <c r="M47">
+        <v>99.26</v>
+      </c>
+      <c r="N47">
+        <v>98.37</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A48" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B48" s="3">
+        <v>0.65</v>
+      </c>
+      <c r="C48" s="3">
+        <v>30</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E48" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F48" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G48" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="H48" s="5">
+        <v>28</v>
+      </c>
+      <c r="I48" s="5">
+        <v>64</v>
+      </c>
+      <c r="J48">
+        <v>100</v>
+      </c>
+      <c r="K48">
+        <v>99.62</v>
+      </c>
+      <c r="L48">
+        <v>100</v>
+      </c>
+      <c r="M48">
+        <v>99.39</v>
+      </c>
+      <c r="N48">
+        <v>98.78</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A49" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B49" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="C49" s="3">
+        <v>30</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E49" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G49" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="H49" s="5">
+        <v>28</v>
+      </c>
+      <c r="I49" s="5">
+        <v>64</v>
+      </c>
+      <c r="J49">
+        <v>100</v>
+      </c>
+      <c r="K49">
+        <v>99.68</v>
+      </c>
+      <c r="L49">
+        <v>100</v>
+      </c>
+      <c r="M49">
+        <v>99.44</v>
+      </c>
+      <c r="N49">
+        <v>98.84</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="F50" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G50" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="H50" s="5">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="J1:L1"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Making next experiments with prediction code
</commit_message>
<xml_diff>
--- a/MBIST input test run output/Changes In HTM Parameters.xlsx
+++ b/MBIST input test run output/Changes In HTM Parameters.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\source\repos\neocortexapi-classification\MBIST input test run output\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\source\repos\image-classification\MBIST input test run output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3B6D607D-F578-41B6-BEE1-C14BD1182640}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{441186E2-09F6-4F07-BA18-72D5CD0649D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="72">
   <si>
     <t>Local Area Density</t>
   </si>
@@ -226,6 +226,21 @@
   </si>
   <si>
     <t>Exp 38</t>
+  </si>
+  <si>
+    <t>Exp 51</t>
+  </si>
+  <si>
+    <t>Test Image</t>
+  </si>
+  <si>
+    <t>O/P</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Good - No Overlapping between micro and macro </t>
   </si>
 </sst>
 </file>
@@ -592,10 +607,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N50"/>
+  <dimension ref="A1:Q51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" topLeftCell="I40" workbookViewId="0">
+      <selection activeCell="Q40" sqref="Q1:Q1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -611,6 +626,8 @@
     <col min="9" max="9" width="18" customWidth="1"/>
     <col min="13" max="13" width="20.88671875" customWidth="1"/>
     <col min="14" max="14" width="28.6640625" customWidth="1"/>
+    <col min="15" max="15" width="12.109375" customWidth="1"/>
+    <col min="17" max="17" width="45.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -2721,7 +2738,7 @@
         <v>98.78</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
         <v>57</v>
       </c>
@@ -2765,7 +2782,19 @@
         <v>98.84</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A50" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B50" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="C50" s="3">
+        <v>1</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>4</v>
+      </c>
       <c r="F50" s="3" t="s">
         <v>65</v>
       </c>
@@ -2774,6 +2803,50 @@
       </c>
       <c r="H50" s="5">
         <v>28</v>
+      </c>
+      <c r="O50" t="s">
+        <v>68</v>
+      </c>
+      <c r="P50" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="F51" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G51" t="s">
+        <v>67</v>
+      </c>
+      <c r="H51">
+        <v>28</v>
+      </c>
+      <c r="I51">
+        <v>64</v>
+      </c>
+      <c r="J51">
+        <v>76.63</v>
+      </c>
+      <c r="K51">
+        <v>70.510000000000005</v>
+      </c>
+      <c r="L51">
+        <v>72.69</v>
+      </c>
+      <c r="M51">
+        <v>56.04</v>
+      </c>
+      <c r="N51">
+        <v>54.29</v>
+      </c>
+      <c r="O51">
+        <v>5</v>
+      </c>
+      <c r="P51" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q51" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>